<commit_message>
add contact activity doesn't crash anymore if no contact selected - for real this time
</commit_message>
<xml_diff>
--- a/MAuS Checklist.xlsx
+++ b/MAuS Checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joker\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joker\IntelliJIDEAProjects\maus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8160A24C-84E8-44EF-A98C-391F6DA589CB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD37E85E-CE6D-4B07-8CC3-4A89AD630972}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="888" yWindow="-60" windowWidth="45252" windowHeight="26040" xr2:uid="{38B7F3F0-9B65-4F14-8064-291420A5D682}"/>
   </bookViews>
@@ -362,7 +362,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -377,8 +377,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -387,6 +385,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -775,17 +782,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5172CE78-7C69-4F42-8E1F-DDE0E0AFFD57}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.21875" style="2" customWidth="1"/>
     <col min="2" max="2" width="46.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="6"/>
-    <col min="5" max="5" width="92.21875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="10"/>
+    <col min="5" max="5" width="92.21875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -795,10 +802,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6">
+      <c r="C1" s="9">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10">
         <v>1</v>
       </c>
     </row>
@@ -806,10 +813,10 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10">
         <v>1</v>
       </c>
     </row>
@@ -817,10 +824,10 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10">
         <v>1</v>
       </c>
     </row>
@@ -828,10 +835,10 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10">
         <v>1</v>
       </c>
     </row>
@@ -839,10 +846,10 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
         <v>1</v>
       </c>
     </row>
@@ -850,10 +857,10 @@
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="C6" s="9">
+        <v>2</v>
+      </c>
+      <c r="D6" s="10">
         <v>2</v>
       </c>
     </row>
@@ -864,7 +871,7 @@
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>3</v>
       </c>
     </row>
@@ -872,10 +879,10 @@
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="9">
         <v>4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="10">
         <v>4</v>
       </c>
     </row>
@@ -883,7 +890,7 @@
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
         <v>1</v>
       </c>
     </row>
@@ -891,7 +898,7 @@
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="9">
         <v>4</v>
       </c>
     </row>
@@ -902,10 +909,10 @@
       <c r="B11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="C11" s="9">
+        <v>3</v>
+      </c>
+      <c r="D11" s="10">
         <v>3</v>
       </c>
     </row>
@@ -913,10 +920,10 @@
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="10">
         <v>1</v>
       </c>
     </row>
@@ -924,10 +931,10 @@
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="9" t="s">
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -935,10 +942,10 @@
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="10">
         <v>1</v>
       </c>
     </row>
@@ -946,10 +953,10 @@
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="10">
         <v>1</v>
       </c>
     </row>
@@ -957,10 +964,10 @@
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6">
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="D16" s="10">
         <v>1</v>
       </c>
     </row>
@@ -968,10 +975,10 @@
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="C17" s="9">
+        <v>2</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -979,7 +986,7 @@
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="9">
         <v>2</v>
       </c>
     </row>
@@ -987,7 +994,7 @@
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="9">
         <v>1</v>
       </c>
     </row>
@@ -995,7 +1002,7 @@
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1003,7 +1010,7 @@
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1011,7 +1018,7 @@
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1019,7 +1026,7 @@
       <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1027,7 +1034,7 @@
       <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1035,10 +1042,10 @@
       <c r="B25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25" s="6">
+      <c r="C25" s="9">
+        <v>3</v>
+      </c>
+      <c r="D25" s="10">
         <v>3</v>
       </c>
     </row>
@@ -1049,10 +1056,10 @@
       <c r="B26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" s="6">
+      <c r="C26" s="9">
+        <v>1</v>
+      </c>
+      <c r="D26" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1060,10 +1067,10 @@
       <c r="B27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" s="6">
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+      <c r="D27" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1071,10 +1078,10 @@
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="8" t="s">
+      <c r="C28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1082,10 +1089,10 @@
       <c r="B29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="6">
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+      <c r="D29" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1093,10 +1100,10 @@
       <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="6">
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+      <c r="D30" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1104,10 +1111,10 @@
       <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31" s="6">
+      <c r="C31" s="9">
+        <v>2</v>
+      </c>
+      <c r="D31" s="10">
         <v>2</v>
       </c>
     </row>
@@ -1115,13 +1122,13 @@
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C32">
-        <v>3</v>
-      </c>
-      <c r="D32" s="6">
-        <v>1</v>
-      </c>
-      <c r="E32" s="8" t="s">
+      <c r="C32" s="9">
+        <v>3</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1129,7 +1136,7 @@
       <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="9">
         <v>3</v>
       </c>
     </row>
@@ -1137,7 +1144,7 @@
       <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1145,7 +1152,7 @@
       <c r="B35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1156,13 +1163,13 @@
       <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="9">
         <v>4</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="10">
         <v>4</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1170,10 +1177,10 @@
       <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" s="6">
+      <c r="C37" s="9">
+        <v>1</v>
+      </c>
+      <c r="D37" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1181,10 +1188,10 @@
       <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" s="6">
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+      <c r="D38" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1192,10 +1199,10 @@
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39" s="6">
+      <c r="C39" s="9">
+        <v>2</v>
+      </c>
+      <c r="D39" s="10">
         <v>2</v>
       </c>
     </row>
@@ -1203,10 +1210,10 @@
       <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" s="6">
+      <c r="C40" s="9">
+        <v>1</v>
+      </c>
+      <c r="D40" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1214,10 +1221,10 @@
       <c r="B41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C41">
-        <v>3</v>
-      </c>
-      <c r="D41" s="6">
+      <c r="C41" s="9">
+        <v>3</v>
+      </c>
+      <c r="D41" s="10">
         <v>3</v>
       </c>
     </row>
@@ -1225,10 +1232,10 @@
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C42">
-        <v>3</v>
-      </c>
-      <c r="D42" s="6">
+      <c r="C42" s="9">
+        <v>3</v>
+      </c>
+      <c r="D42" s="10">
         <v>3</v>
       </c>
     </row>
@@ -1239,7 +1246,7 @@
       <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="9">
         <v>6</v>
       </c>
     </row>
@@ -1250,10 +1257,10 @@
       <c r="B44" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" s="6">
+      <c r="C44" s="9">
+        <v>1</v>
+      </c>
+      <c r="D44" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1261,10 +1268,10 @@
       <c r="B45" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45" s="6">
+      <c r="C45" s="9">
+        <v>2</v>
+      </c>
+      <c r="D45" s="10">
         <v>2</v>
       </c>
     </row>
@@ -1272,10 +1279,10 @@
       <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C46">
-        <v>3</v>
-      </c>
-      <c r="D46" s="6">
+      <c r="C46" s="9">
+        <v>3</v>
+      </c>
+      <c r="D46" s="10">
         <v>3</v>
       </c>
     </row>
@@ -1283,10 +1290,10 @@
       <c r="B47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
-      <c r="D47" s="6">
+      <c r="C47" s="9">
+        <v>2</v>
+      </c>
+      <c r="D47" s="10">
         <v>2</v>
       </c>
     </row>
@@ -1294,10 +1301,10 @@
       <c r="B48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48" s="6">
+      <c r="C48" s="9">
+        <v>2</v>
+      </c>
+      <c r="D48" s="10">
         <v>2</v>
       </c>
     </row>
@@ -1305,13 +1312,13 @@
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49" s="6">
-        <v>1</v>
-      </c>
-      <c r="E49" s="8" t="s">
+      <c r="C49" s="9">
+        <v>2</v>
+      </c>
+      <c r="D49" s="10">
+        <v>1</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1319,7 +1326,7 @@
       <c r="B50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1327,7 +1334,7 @@
       <c r="B51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="9">
         <v>3</v>
       </c>
     </row>
@@ -1335,7 +1342,7 @@
       <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1343,25 +1350,25 @@
       <c r="B53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" s="6">
+      <c r="C53" s="9">
+        <v>1</v>
+      </c>
+      <c r="D53" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
-      <c r="C55" s="7">
+      <c r="C55" s="11">
         <f>SUM(C1:C53)</f>
         <v>100</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D55" s="11">
         <f>SUM(D1:D53)</f>
         <v>55</v>
       </c>
-      <c r="E55" s="10"/>
+      <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>

<commit_message>
Login button only clickable if values for email and password entered. (60/100)
</commit_message>
<xml_diff>
--- a/MAuS Checklist.xlsx
+++ b/MAuS Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joker\IntelliJIDEAProjects\maus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D311C46-6837-4D60-89CF-ECD884B5ED70}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A550FE23-73FF-4653-84D8-840367099ECD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="888" yWindow="-60" windowWidth="45252" windowHeight="26040" xr2:uid="{38B7F3F0-9B65-4F14-8064-291420A5D682}"/>
+    <workbookView xWindow="-16275" yWindow="-6000" windowWidth="16350" windowHeight="28350" tabRatio="396" xr2:uid="{38B7F3F0-9B65-4F14-8064-291420A5D682}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Datenmodell</t>
   </si>
@@ -216,9 +216,6 @@
   <si>
     <t>Als Banner?
 Bei uns wird gerade nur eine Warnung angezeigt, wenn auch das Passwort nicht genügt…</t>
-  </si>
-  <si>
-    <t>Der muss noch disabled werden</t>
   </si>
   <si>
     <t>den Namen</t>
@@ -779,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5172CE78-7C69-4F42-8E1F-DDE0E0AFFD57}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -975,8 +972,8 @@
       <c r="C17" s="9">
         <v>2</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>58</v>
+      <c r="D17" s="10">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1051,7 +1048,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -1062,7 +1059,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="9">
         <v>1</v>
@@ -1079,12 +1076,12 @@
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -1126,7 +1123,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1167,7 +1164,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1363,7 +1360,7 @@
       </c>
       <c r="D55" s="11">
         <f>SUM(D1:D53)</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E55" s="8"/>
     </row>

</xml_diff>

<commit_message>
Swipe to toggle done in TodoListActivity (62/100)
</commit_message>
<xml_diff>
--- a/MAuS Checklist.xlsx
+++ b/MAuS Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joker\IntelliJIDEAProjects\maus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A550FE23-73FF-4653-84D8-840367099ECD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B8EE04-D83F-41EA-A326-D40975109104}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16275" yWindow="-6000" windowWidth="16350" windowHeight="28350" tabRatio="396" xr2:uid="{38B7F3F0-9B65-4F14-8064-291420A5D682}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Datenmodell</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>Sollte schnell machbar sein</t>
-  </si>
-  <si>
-    <t>Erledigtsein schient noch nicht zu funktionieren</t>
   </si>
   <si>
     <t>Fehlt da was?</t>
@@ -776,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5172CE78-7C69-4F42-8E1F-DDE0E0AFFD57}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -1024,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1033,6 +1030,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="B25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1044,9 +1044,6 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="B26" s="1" t="s">
         <v>58</v>
       </c>
@@ -1120,10 +1117,7 @@
         <v>3</v>
       </c>
       <c r="D32" s="10">
-        <v>1</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1164,7 +1158,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1360,7 +1354,7 @@
       </c>
       <c r="D55" s="11">
         <f>SUM(D1:D53)</f>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E55" s="8"/>
     </row>

</xml_diff>

<commit_message>
display done or not done in TodoListActivity (63/100)
</commit_message>
<xml_diff>
--- a/MAuS Checklist.xlsx
+++ b/MAuS Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joker\IntelliJIDEAProjects\maus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F46EA7C-0A54-4942-A813-AA37D4919431}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C00C92-606C-4E10-BB26-80F25218F092}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="888" yWindow="-60" windowWidth="45252" windowHeight="26040" tabRatio="396" xr2:uid="{38B7F3F0-9B65-4F14-8064-291420A5D682}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Datenmodell</t>
   </si>
@@ -225,9 +225,6 @@
   </si>
   <si>
     <t>die Wichtigkeit</t>
-  </si>
-  <si>
-    <t>Sollte schnell machbar sein</t>
   </si>
   <si>
     <t>Fehlt da was?</t>
@@ -376,14 +373,7 @@
     <cellStyle name="Ergebnis" xfId="2" builtinId="25"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -771,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5172CE78-7C69-4F42-8E1F-DDE0E0AFFD57}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -960,7 +950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -971,7 +961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -979,7 +969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
@@ -987,7 +977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
@@ -995,7 +985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1003,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1011,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1019,7 +1009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1027,7 +1017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -1041,7 +1031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>58</v>
       </c>
@@ -1052,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>59</v>
       </c>
@@ -1063,18 +1053,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="9">
         <v>1</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1085,7 +1075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1096,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1107,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1156,7 +1146,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1352,14 +1342,14 @@
       </c>
       <c r="D55" s="9">
         <f>SUM(D1:D53)</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>C1&lt;&gt;D1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix highlight overdue (65/100)
</commit_message>
<xml_diff>
--- a/MAuS Checklist.xlsx
+++ b/MAuS Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joker\IntelliJIDEAProjects\maus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B80E02D-6C4B-461C-A808-1404A4D84DCA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED169A2-96EB-4204-9C5F-70E2B499D702}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="888" yWindow="-60" windowWidth="45252" windowHeight="26040" tabRatio="396" xr2:uid="{38B7F3F0-9B65-4F14-8064-291420A5D682}"/>
+    <workbookView xWindow="-16275" yWindow="-6000" windowWidth="16350" windowHeight="28350" tabRatio="396" xr2:uid="{38B7F3F0-9B65-4F14-8064-291420A5D682}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Datenmodell</t>
   </si>
@@ -214,20 +214,23 @@
     <t>Erlauben Sie dem Nutzer, Todos optional mit einer Menge von Kontakten zu verknüpfen.</t>
   </si>
   <si>
+    <t>den Namen</t>
+  </si>
+  <si>
+    <t>das Fälligkeitsdatum</t>
+  </si>
+  <si>
+    <t>die Wichtigkeit</t>
+  </si>
+  <si>
+    <t>Ist hier nur von der Eingabe die Rede oder auch von der Funktionalität? Dann weniger Punkte…</t>
+  </si>
+  <si>
     <t>Als Banner?
-Bei uns wird gerade nur eine Warnung angezeigt, wenn auch das Passwort nicht genügt…</t>
-  </si>
-  <si>
-    <t>den Namen</t>
-  </si>
-  <si>
-    <t>das Fälligkeitsdatum</t>
-  </si>
-  <si>
-    <t>die Wichtigkeit</t>
-  </si>
-  <si>
-    <t>Fehlt da was?</t>
+Was heißt "dauerhaft sichtbar"?</t>
+  </si>
+  <si>
+    <t>Uhrzeit wird immer als AM gespiechert.</t>
   </si>
 </sst>
 </file>
@@ -373,14 +376,7 @@
     <cellStyle name="Ergebnis" xfId="2" builtinId="25"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -768,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5172CE78-7C69-4F42-8E1F-DDE0E0AFFD57}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -901,6 +897,9 @@
       <c r="D11" s="9">
         <v>3</v>
       </c>
+      <c r="E11" s="6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
@@ -921,7 +920,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1040,7 +1039,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -1051,7 +1050,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="9">
         <v>1</v>
@@ -1073,7 +1072,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -1138,6 +1137,12 @@
       <c r="C35" s="9">
         <v>2</v>
       </c>
+      <c r="D35" s="9">
+        <v>2</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
@@ -1151,9 +1156,6 @@
       </c>
       <c r="D36" s="9">
         <v>4</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1349,14 +1351,14 @@
       </c>
       <c r="D55" s="9">
         <f>SUM(D1:D53)</f>
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>C1&lt;&gt;D1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>